<commit_message>
correct column A name
</commit_message>
<xml_diff>
--- a/cost recovery record from 2025.xlsx
+++ b/cost recovery record from 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsrisai\Documents\TPSR core inventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F302298B-80AD-4DB1-96AB-145E4FDA562B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283004C1-E160-45E8-8ADD-D48A8FB3E4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="555" windowWidth="21600" windowHeight="11595" xr2:uid="{A65C8BF4-CB96-401D-8F12-F9A2BDA0DEB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A65C8BF4-CB96-401D-8F12-F9A2BDA0DEB4}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -89,13 +89,13 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>Requester_name</t>
-  </si>
-  <si>
     <t>Cost_Recovery</t>
   </si>
   <si>
     <t>Required_Date</t>
+  </si>
+  <si>
+    <t>Requester_Name</t>
   </si>
 </sst>
 </file>
@@ -485,9 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D03DD13-4E3A-4CD6-879D-A1B2A04A1C17}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -505,16 +503,16 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>9</v>

</xml_diff>